<commit_message>
Cotización Gente de Talento
</commit_message>
<xml_diff>
--- a/Varios/Proforma/Proforma.xlsx
+++ b/Varios/Proforma/Proforma.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar.gamboa\Documents\Github\Website\Varios\Proforma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c0abcc15bdc5c59/GitHub/Website/Varios/Proforma/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_C686E72F8702C360D548D0B2E91953FC2BD2E2E2" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17C17C3F-B871-48F5-B5F7-F5B7CD079B6A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="0"/>
+  <calcPr calcId="191029" iterateDelta="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,16 +50,16 @@
     <t>detalle</t>
   </si>
   <si>
-    <t>Cálculo de indicadores para la metodología de medición del IBINA</t>
-  </si>
-  <si>
     <t>servicio</t>
+  </si>
+  <si>
+    <t>Servicio de consultoría estadística.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,11 +404,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,16 +432,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1392888</v>
+        <v>33000</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>